<commit_message>
Science Nodes now require Electronics Blue Sky, Solids Restructure (new node and made cheaper)
</commit_message>
<xml_diff>
--- a/Source/Tech Tree/Tree Years.xlsx
+++ b/Source/Tech Tree/Tree Years.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pap\Dropbox\GAMES\KSP\Git\RP-0\Source\Tech Tree\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B95EE43-62CE-4E12-9120-B9F2E642A557}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CAF0279-D200-473F-9CFD-474EB4A4EE41}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="33090" yWindow="1785" windowWidth="18000" windowHeight="9360" activeTab="1" xr2:uid="{73CA1BD0-04E5-4D1A-9F47-B0D01E7997A1}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{73CA1BD0-04E5-4D1A-9F47-B0D01E7997A1}"/>
   </bookViews>
   <sheets>
     <sheet name="RAW" sheetId="2" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5917" uniqueCount="312">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5917" uniqueCount="313">
   <si>
     <t>GROUP</t>
   </si>
@@ -965,6 +965,9 @@
   </si>
   <si>
     <t>(blank)</t>
+  </si>
+  <si>
+    <t>basicSolids</t>
   </si>
 </sst>
 </file>
@@ -8060,7 +8063,7 @@
   <dimension ref="A1:C1963"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B711" sqref="B711"/>
+      <selection activeCell="B905" sqref="B905"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -18019,7 +18022,7 @@
         <v>1952</v>
       </c>
       <c r="B905" t="s">
-        <v>154</v>
+        <v>312</v>
       </c>
       <c r="C905" t="s">
         <v>153</v>
@@ -18030,7 +18033,7 @@
         <v>1953</v>
       </c>
       <c r="B906" t="s">
-        <v>154</v>
+        <v>312</v>
       </c>
       <c r="C906" t="s">
         <v>153</v>
@@ -18041,7 +18044,7 @@
         <v>1954</v>
       </c>
       <c r="B907" t="s">
-        <v>154</v>
+        <v>312</v>
       </c>
       <c r="C907" t="s">
         <v>153</v>
@@ -18052,7 +18055,7 @@
         <v>1955</v>
       </c>
       <c r="B908" t="s">
-        <v>154</v>
+        <v>312</v>
       </c>
       <c r="C908" t="s">
         <v>153</v>

</xml_diff>

<commit_message>
Add missing comms tech nodes to year mapping files
</commit_message>
<xml_diff>
--- a/Source/Tech Tree/Tree Years.xlsx
+++ b/Source/Tech Tree/Tree Years.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pap\Dropbox\GAMES\KSP\Git\RP-0\Source\Tech Tree\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\siim\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CAF0279-D200-473F-9CFD-474EB4A4EE41}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01127C48-2EE7-4688-98D4-1807BF7743F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{73CA1BD0-04E5-4D1A-9F47-B0D01E7997A1}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{73CA1BD0-04E5-4D1A-9F47-B0D01E7997A1}"/>
   </bookViews>
   <sheets>
     <sheet name="RAW" sheetId="2" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5917" uniqueCount="313">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5917" uniqueCount="315">
   <si>
     <t>GROUP</t>
   </si>
@@ -968,6 +968,12 @@
   </si>
   <si>
     <t>basicSolids</t>
+  </si>
+  <si>
+    <t>highDataRateComms</t>
+  </si>
+  <si>
+    <t>digitalComms</t>
   </si>
 </sst>
 </file>
@@ -1104,7 +1110,7 @@
   <autoFilter ref="A1:C1963" xr:uid="{9BA48B2D-B23C-4546-9267-C4BE6CED0FC8}">
     <filterColumn colId="2">
       <filters>
-        <filter val="Solid"/>
+        <filter val="Comms"/>
       </filters>
     </filterColumn>
   </autoFilter>
@@ -1416,8 +1422,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C174049B-F960-49D1-93D8-1CC39D0C8787}">
   <dimension ref="A1:U107"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="S13" sqref="S13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1950,7 +1956,7 @@
         <v>220</v>
       </c>
       <c r="S11" s="6" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="T11" s="6" t="s">
         <v>263</v>
@@ -2046,7 +2052,7 @@
         <v>248</v>
       </c>
       <c r="S13" s="6" t="s">
-        <v>264</v>
+        <v>314</v>
       </c>
       <c r="T13" s="9" t="s">
         <v>278</v>
@@ -2099,7 +2105,7 @@
         <v>248</v>
       </c>
       <c r="S14" s="6" t="s">
-        <v>264</v>
+        <v>314</v>
       </c>
       <c r="T14" s="6" t="s">
         <v>278</v>
@@ -3081,7 +3087,7 @@
         <v>253</v>
       </c>
       <c r="S30" s="6" t="s">
-        <v>268</v>
+        <v>313</v>
       </c>
       <c r="T30" s="6" t="s">
         <v>283</v>
@@ -3144,7 +3150,7 @@
         <v>253</v>
       </c>
       <c r="S31" s="6" t="s">
-        <v>268</v>
+        <v>313</v>
       </c>
       <c r="T31" s="6" t="s">
         <v>283</v>
@@ -3207,7 +3213,7 @@
         <v>253</v>
       </c>
       <c r="S32" s="6" t="s">
-        <v>268</v>
+        <v>313</v>
       </c>
       <c r="T32" s="6" t="s">
         <v>283</v>
@@ -3270,7 +3276,7 @@
         <v>253</v>
       </c>
       <c r="S33" s="6" t="s">
-        <v>268</v>
+        <v>313</v>
       </c>
       <c r="T33" s="6" t="s">
         <v>283</v>
@@ -3333,7 +3339,7 @@
         <v>253</v>
       </c>
       <c r="S34" s="6" t="s">
-        <v>268</v>
+        <v>313</v>
       </c>
       <c r="T34" s="6" t="s">
         <v>283</v>
@@ -8055,6 +8061,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -8063,7 +8070,7 @@
   <dimension ref="A1:C1963"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B905" sqref="B905"/>
+      <selection activeCell="E1658" sqref="E1658"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -17984,7 +17991,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="902" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="902" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A902">
         <v>0</v>
       </c>
@@ -17995,7 +18002,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="903" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="903" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A903">
         <v>1950</v>
       </c>
@@ -18006,7 +18013,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="904" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="904" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A904">
         <v>1951</v>
       </c>
@@ -18017,7 +18024,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="905" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="905" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A905">
         <v>1952</v>
       </c>
@@ -18028,7 +18035,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="906" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="906" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A906">
         <v>1953</v>
       </c>
@@ -18039,7 +18046,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="907" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="907" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A907">
         <v>1954</v>
       </c>
@@ -18050,7 +18057,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="908" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="908" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A908">
         <v>1955</v>
       </c>
@@ -18061,7 +18068,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="909" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="909" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A909">
         <v>1956</v>
       </c>
@@ -18072,7 +18079,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="910" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="910" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A910">
         <v>1957</v>
       </c>
@@ -18083,7 +18090,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="911" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="911" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A911">
         <v>1958</v>
       </c>
@@ -18094,7 +18101,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="912" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="912" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A912">
         <v>1959</v>
       </c>
@@ -18105,7 +18112,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="913" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="913" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A913">
         <v>1960</v>
       </c>
@@ -18116,7 +18123,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="914" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="914" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A914">
         <v>1961</v>
       </c>
@@ -18127,7 +18134,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="915" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="915" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A915">
         <v>1962</v>
       </c>
@@ -18138,7 +18145,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="916" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="916" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A916">
         <v>1963</v>
       </c>
@@ -18149,7 +18156,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="917" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="917" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A917">
         <v>1964</v>
       </c>
@@ -18160,7 +18167,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="918" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="918" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A918">
         <v>1965</v>
       </c>
@@ -18171,7 +18178,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="919" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="919" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A919">
         <v>1966</v>
       </c>
@@ -18182,7 +18189,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="920" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="920" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A920">
         <v>1967</v>
       </c>
@@ -18193,7 +18200,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="921" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="921" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A921">
         <v>1968</v>
       </c>
@@ -18204,7 +18211,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="922" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="922" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A922">
         <v>1969</v>
       </c>
@@ -18215,7 +18222,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="923" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="923" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A923">
         <v>1970</v>
       </c>
@@ -18226,7 +18233,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="924" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="924" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A924">
         <v>1971</v>
       </c>
@@ -18237,7 +18244,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="925" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="925" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A925">
         <v>1972</v>
       </c>
@@ -18248,7 +18255,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="926" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="926" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A926">
         <v>1973</v>
       </c>
@@ -18259,7 +18266,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="927" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="927" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A927">
         <v>1974</v>
       </c>
@@ -18270,7 +18277,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="928" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="928" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A928">
         <v>1975</v>
       </c>
@@ -18281,7 +18288,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="929" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="929" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A929">
         <v>1976</v>
       </c>
@@ -18292,7 +18299,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="930" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="930" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A930">
         <v>1977</v>
       </c>
@@ -18303,7 +18310,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="931" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="931" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A931">
         <v>1978</v>
       </c>
@@ -18314,7 +18321,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="932" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="932" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A932">
         <v>1979</v>
       </c>
@@ -18325,7 +18332,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="933" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="933" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A933">
         <v>1980</v>
       </c>
@@ -18336,7 +18343,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="934" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="934" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A934">
         <v>1981</v>
       </c>
@@ -18347,7 +18354,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="935" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="935" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A935">
         <v>1982</v>
       </c>
@@ -18358,7 +18365,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="936" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="936" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A936">
         <v>1983</v>
       </c>
@@ -18369,7 +18376,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="937" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="937" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A937">
         <v>1984</v>
       </c>
@@ -18380,7 +18387,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="938" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="938" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A938">
         <v>1985</v>
       </c>
@@ -18391,7 +18398,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="939" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="939" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A939">
         <v>1986</v>
       </c>
@@ -18402,7 +18409,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="940" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="940" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A940">
         <v>1987</v>
       </c>
@@ -18413,7 +18420,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="941" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="941" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A941">
         <v>1988</v>
       </c>
@@ -18424,7 +18431,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="942" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="942" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A942">
         <v>1989</v>
       </c>
@@ -18435,7 +18442,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="943" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="943" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A943">
         <v>1990</v>
       </c>
@@ -18446,7 +18453,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="944" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="944" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A944">
         <v>1991</v>
       </c>
@@ -18457,7 +18464,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="945" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="945" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A945">
         <v>1992</v>
       </c>
@@ -18468,7 +18475,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="946" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="946" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A946">
         <v>1993</v>
       </c>
@@ -18479,7 +18486,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="947" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="947" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A947">
         <v>1994</v>
       </c>
@@ -18490,7 +18497,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="948" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="948" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A948">
         <v>1995</v>
       </c>
@@ -18501,7 +18508,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="949" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="949" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A949">
         <v>1996</v>
       </c>
@@ -18512,7 +18519,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="950" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="950" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A950">
         <v>1997</v>
       </c>
@@ -18523,7 +18530,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="951" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="951" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A951">
         <v>1998</v>
       </c>
@@ -18534,7 +18541,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="952" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="952" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A952">
         <v>1999</v>
       </c>
@@ -18545,7 +18552,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="953" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="953" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A953">
         <v>2000</v>
       </c>
@@ -18556,7 +18563,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="954" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="954" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A954">
         <v>2001</v>
       </c>
@@ -18567,7 +18574,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="955" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="955" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A955">
         <v>2002</v>
       </c>
@@ -18578,7 +18585,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="956" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="956" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A956">
         <v>2003</v>
       </c>
@@ -18589,7 +18596,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="957" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="957" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A957">
         <v>2004</v>
       </c>
@@ -18600,7 +18607,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="958" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="958" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A958">
         <v>2005</v>
       </c>
@@ -18611,7 +18618,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="959" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="959" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A959">
         <v>2006</v>
       </c>
@@ -18622,7 +18629,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="960" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="960" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A960">
         <v>2007</v>
       </c>
@@ -18633,7 +18640,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="961" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="961" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A961">
         <v>2008</v>
       </c>
@@ -18644,7 +18651,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="962" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="962" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A962">
         <v>2009</v>
       </c>
@@ -18655,7 +18662,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="963" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="963" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A963">
         <v>2010</v>
       </c>
@@ -18666,7 +18673,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="964" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="964" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A964">
         <v>2011</v>
       </c>
@@ -18677,7 +18684,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="965" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="965" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A965">
         <v>2012</v>
       </c>
@@ -18688,7 +18695,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="966" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="966" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A966">
         <v>2013</v>
       </c>
@@ -18699,7 +18706,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="967" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="967" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A967">
         <v>2014</v>
       </c>
@@ -18710,7 +18717,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="968" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="968" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A968">
         <v>2015</v>
       </c>
@@ -18721,7 +18728,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="969" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="969" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A969">
         <v>2016</v>
       </c>
@@ -18732,7 +18739,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="970" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="970" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A970">
         <v>2017</v>
       </c>
@@ -18743,7 +18750,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="971" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="971" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A971">
         <v>2018</v>
       </c>
@@ -18754,7 +18761,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="972" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="972" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A972">
         <v>2019</v>
       </c>
@@ -18765,7 +18772,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="973" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="973" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A973">
         <v>2020</v>
       </c>
@@ -18776,7 +18783,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="974" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="974" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A974">
         <v>2021</v>
       </c>
@@ -18787,7 +18794,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="975" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="975" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A975">
         <v>2022</v>
       </c>
@@ -18798,7 +18805,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="976" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="976" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A976">
         <v>2023</v>
       </c>
@@ -18809,7 +18816,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="977" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="977" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A977">
         <v>2024</v>
       </c>
@@ -18820,7 +18827,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="978" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="978" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A978">
         <v>2025</v>
       </c>
@@ -18831,7 +18838,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="979" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="979" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A979">
         <v>2026</v>
       </c>
@@ -18842,7 +18849,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="980" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="980" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A980">
         <v>2027</v>
       </c>
@@ -18853,7 +18860,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="981" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="981" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A981">
         <v>2028</v>
       </c>
@@ -18864,7 +18871,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="982" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="982" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A982">
         <v>2029</v>
       </c>
@@ -18875,7 +18882,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="983" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="983" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A983">
         <v>2030</v>
       </c>
@@ -18886,7 +18893,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="984" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="984" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A984">
         <v>2031</v>
       </c>
@@ -18897,7 +18904,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="985" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="985" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A985">
         <v>2032</v>
       </c>
@@ -18908,7 +18915,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="986" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="986" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A986">
         <v>2033</v>
       </c>
@@ -18919,7 +18926,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="987" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="987" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A987">
         <v>2034</v>
       </c>
@@ -18930,7 +18937,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="988" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="988" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A988">
         <v>2035</v>
       </c>
@@ -18941,7 +18948,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="989" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="989" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A989">
         <v>2036</v>
       </c>
@@ -18952,7 +18959,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="990" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="990" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A990">
         <v>2037</v>
       </c>
@@ -18963,7 +18970,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="991" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="991" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A991">
         <v>2038</v>
       </c>
@@ -18974,7 +18981,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="992" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="992" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A992">
         <v>2039</v>
       </c>
@@ -18985,7 +18992,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="993" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="993" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A993">
         <v>2040</v>
       </c>
@@ -18996,7 +19003,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="994" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="994" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A994">
         <v>2041</v>
       </c>
@@ -19007,7 +19014,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="995" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="995" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A995">
         <v>2042</v>
       </c>
@@ -19018,7 +19025,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="996" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="996" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A996">
         <v>2043</v>
       </c>
@@ -19029,7 +19036,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="997" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="997" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A997">
         <v>2044</v>
       </c>
@@ -19040,7 +19047,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="998" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="998" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A998">
         <v>2045</v>
       </c>
@@ -19051,7 +19058,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="999" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="999" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A999">
         <v>2046</v>
       </c>
@@ -19062,7 +19069,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="1000" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1000" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1000">
         <v>2047</v>
       </c>
@@ -19073,7 +19080,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="1001" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1001" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1001">
         <v>2048</v>
       </c>
@@ -19084,7 +19091,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="1002" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1002" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1002">
         <v>2049</v>
       </c>
@@ -19095,7 +19102,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="1003" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1003" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1003">
         <v>2050</v>
       </c>
@@ -19106,7 +19113,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="1004" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1004" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1004">
         <v>2051</v>
       </c>
@@ -19117,7 +19124,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="1005" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1005" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1005">
         <v>2100</v>
       </c>
@@ -19128,7 +19135,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="1006" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1006" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1006">
         <v>2150</v>
       </c>
@@ -19139,7 +19146,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="1007" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1007" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1007" t="s">
         <v>1</v>
       </c>
@@ -26245,7 +26252,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="1653" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1653" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1653">
         <v>0</v>
       </c>
@@ -26256,7 +26263,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="1654" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1654" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1654">
         <v>1956</v>
       </c>
@@ -26267,18 +26274,18 @@
         <v>262</v>
       </c>
     </row>
-    <row r="1655" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1655" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1655">
         <v>1957</v>
       </c>
       <c r="B1655" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="C1655" t="s">
         <v>262</v>
       </c>
     </row>
-    <row r="1656" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1656" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1656">
         <v>1958</v>
       </c>
@@ -26289,29 +26296,29 @@
         <v>262</v>
       </c>
     </row>
-    <row r="1657" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1657" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1657">
         <v>1959</v>
       </c>
       <c r="B1657" t="s">
-        <v>264</v>
+        <v>314</v>
       </c>
       <c r="C1657" t="s">
         <v>262</v>
       </c>
     </row>
-    <row r="1658" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1658" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1658">
         <v>1960</v>
       </c>
       <c r="B1658" t="s">
-        <v>264</v>
+        <v>314</v>
       </c>
       <c r="C1658" t="s">
         <v>262</v>
       </c>
     </row>
-    <row r="1659" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1659" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1659">
         <v>1961</v>
       </c>
@@ -26322,7 +26329,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="1660" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1660" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1660">
         <v>1962</v>
       </c>
@@ -26333,7 +26340,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="1661" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1661" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1661">
         <v>1963</v>
       </c>
@@ -26344,7 +26351,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="1662" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1662" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1662">
         <v>1964</v>
       </c>
@@ -26355,7 +26362,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="1663" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1663" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1663">
         <v>1965</v>
       </c>
@@ -26366,7 +26373,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="1664" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1664" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1664">
         <v>1966</v>
       </c>
@@ -26377,7 +26384,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="1665" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1665" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1665">
         <v>1967</v>
       </c>
@@ -26388,7 +26395,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="1666" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1666" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1666">
         <v>1968</v>
       </c>
@@ -26399,7 +26406,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="1667" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1667" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1667">
         <v>1969</v>
       </c>
@@ -26410,7 +26417,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="1668" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1668" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1668">
         <v>1970</v>
       </c>
@@ -26421,7 +26428,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="1669" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1669" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1669">
         <v>1971</v>
       </c>
@@ -26432,7 +26439,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="1670" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1670" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1670">
         <v>1972</v>
       </c>
@@ -26443,7 +26450,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="1671" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1671" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1671">
         <v>1973</v>
       </c>
@@ -26454,7 +26461,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="1672" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1672" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1672">
         <v>1974</v>
       </c>
@@ -26465,7 +26472,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="1673" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1673" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1673">
         <v>1975</v>
       </c>
@@ -26476,62 +26483,62 @@
         <v>262</v>
       </c>
     </row>
-    <row r="1674" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1674" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1674">
         <v>1976</v>
       </c>
       <c r="B1674" t="s">
-        <v>268</v>
+        <v>313</v>
       </c>
       <c r="C1674" t="s">
         <v>262</v>
       </c>
     </row>
-    <row r="1675" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1675" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1675">
         <v>1977</v>
       </c>
       <c r="B1675" t="s">
-        <v>268</v>
+        <v>313</v>
       </c>
       <c r="C1675" t="s">
         <v>262</v>
       </c>
     </row>
-    <row r="1676" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1676" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1676">
         <v>1978</v>
       </c>
       <c r="B1676" t="s">
-        <v>268</v>
+        <v>313</v>
       </c>
       <c r="C1676" t="s">
         <v>262</v>
       </c>
     </row>
-    <row r="1677" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1677" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1677">
         <v>1979</v>
       </c>
       <c r="B1677" t="s">
-        <v>268</v>
+        <v>313</v>
       </c>
       <c r="C1677" t="s">
         <v>262</v>
       </c>
     </row>
-    <row r="1678" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1678" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1678">
         <v>1980</v>
       </c>
       <c r="B1678" t="s">
-        <v>268</v>
+        <v>313</v>
       </c>
       <c r="C1678" t="s">
         <v>262</v>
       </c>
     </row>
-    <row r="1679" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1679" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1679">
         <v>1981</v>
       </c>
@@ -26542,7 +26549,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="1680" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1680" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1680">
         <v>1982</v>
       </c>
@@ -26553,7 +26560,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="1681" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1681" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1681">
         <v>1983</v>
       </c>
@@ -26564,7 +26571,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="1682" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1682" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1682">
         <v>1984</v>
       </c>
@@ -26575,7 +26582,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="1683" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1683" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1683">
         <v>1985</v>
       </c>
@@ -26586,7 +26593,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="1684" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1684" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1684">
         <v>1986</v>
       </c>
@@ -26597,7 +26604,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="1685" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1685" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1685">
         <v>1987</v>
       </c>
@@ -26608,7 +26615,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="1686" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1686" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1686">
         <v>1988</v>
       </c>
@@ -26619,7 +26626,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="1687" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1687" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1687">
         <v>1989</v>
       </c>
@@ -26630,7 +26637,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="1688" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1688" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1688">
         <v>1990</v>
       </c>
@@ -26641,7 +26648,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="1689" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1689" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1689">
         <v>1991</v>
       </c>
@@ -26652,7 +26659,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="1690" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1690" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1690">
         <v>1992</v>
       </c>
@@ -26663,7 +26670,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="1691" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1691" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1691">
         <v>1993</v>
       </c>
@@ -26674,7 +26681,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="1692" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1692" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1692">
         <v>1994</v>
       </c>
@@ -26685,7 +26692,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="1693" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1693" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1693">
         <v>1995</v>
       </c>
@@ -26696,7 +26703,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="1694" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1694" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1694">
         <v>1996</v>
       </c>
@@ -26707,7 +26714,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="1695" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1695" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1695">
         <v>1997</v>
       </c>
@@ -26718,7 +26725,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="1696" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1696" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1696">
         <v>1998</v>
       </c>
@@ -26729,7 +26736,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="1697" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1697" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1697">
         <v>1999</v>
       </c>
@@ -26740,7 +26747,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="1698" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1698" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1698">
         <v>2000</v>
       </c>
@@ -26751,7 +26758,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="1699" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1699" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1699">
         <v>2001</v>
       </c>
@@ -26762,7 +26769,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="1700" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1700" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1700">
         <v>2002</v>
       </c>
@@ -26773,7 +26780,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="1701" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1701" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1701">
         <v>2003</v>
       </c>
@@ -26784,7 +26791,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="1702" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1702" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1702">
         <v>2004</v>
       </c>
@@ -26795,7 +26802,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="1703" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1703" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1703">
         <v>2005</v>
       </c>
@@ -26806,7 +26813,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="1704" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1704" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1704">
         <v>2006</v>
       </c>
@@ -26817,7 +26824,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="1705" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1705" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1705">
         <v>2007</v>
       </c>
@@ -26828,7 +26835,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="1706" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1706" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1706">
         <v>2008</v>
       </c>
@@ -26839,7 +26846,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="1707" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1707" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1707">
         <v>2009</v>
       </c>
@@ -26850,7 +26857,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="1708" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1708" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1708">
         <v>2010</v>
       </c>
@@ -26861,7 +26868,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="1709" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1709" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1709">
         <v>2011</v>
       </c>
@@ -26872,7 +26879,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="1710" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1710" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1710">
         <v>2012</v>
       </c>
@@ -26883,7 +26890,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="1711" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1711" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1711">
         <v>2013</v>
       </c>
@@ -26894,7 +26901,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="1712" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1712" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1712">
         <v>2014</v>
       </c>
@@ -26905,7 +26912,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="1713" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1713" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1713">
         <v>2015</v>
       </c>
@@ -26916,7 +26923,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="1714" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1714" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1714">
         <v>2016</v>
       </c>
@@ -26927,7 +26934,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="1715" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1715" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1715">
         <v>2017</v>
       </c>
@@ -26938,7 +26945,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="1716" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1716" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1716">
         <v>2018</v>
       </c>
@@ -26949,7 +26956,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="1717" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1717" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1717">
         <v>2019</v>
       </c>
@@ -26960,7 +26967,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="1718" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1718" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1718">
         <v>2020</v>
       </c>
@@ -26971,7 +26978,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="1719" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1719" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1719">
         <v>2021</v>
       </c>
@@ -26982,7 +26989,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="1720" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1720" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1720">
         <v>2022</v>
       </c>
@@ -26993,7 +27000,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="1721" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1721" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1721">
         <v>2023</v>
       </c>
@@ -27004,7 +27011,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="1722" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1722" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1722">
         <v>2024</v>
       </c>
@@ -27015,7 +27022,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="1723" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1723" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1723">
         <v>2025</v>
       </c>
@@ -27026,7 +27033,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="1724" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1724" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1724">
         <v>2026</v>
       </c>
@@ -27037,7 +27044,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="1725" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1725" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1725">
         <v>2027</v>
       </c>
@@ -27048,7 +27055,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="1726" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1726" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1726">
         <v>2028</v>
       </c>
@@ -27059,7 +27066,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="1727" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1727" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1727">
         <v>2029</v>
       </c>
@@ -27070,7 +27077,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="1728" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1728" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1728">
         <v>2030</v>
       </c>
@@ -27081,7 +27088,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="1729" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1729" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1729">
         <v>2031</v>
       </c>
@@ -27092,7 +27099,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="1730" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1730" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1730">
         <v>2032</v>
       </c>
@@ -27103,7 +27110,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="1731" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1731" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1731">
         <v>2033</v>
       </c>
@@ -27114,7 +27121,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="1732" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1732" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1732">
         <v>2034</v>
       </c>
@@ -27125,7 +27132,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="1733" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1733" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1733">
         <v>2035</v>
       </c>
@@ -27136,7 +27143,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="1734" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1734" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1734">
         <v>2036</v>
       </c>
@@ -27147,7 +27154,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="1735" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1735" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1735">
         <v>2037</v>
       </c>
@@ -27158,7 +27165,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="1736" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1736" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1736">
         <v>2038</v>
       </c>
@@ -27169,7 +27176,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="1737" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1737" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1737">
         <v>2039</v>
       </c>
@@ -27180,7 +27187,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="1738" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1738" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1738">
         <v>2040</v>
       </c>
@@ -27191,7 +27198,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="1739" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1739" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1739">
         <v>2041</v>
       </c>
@@ -27202,7 +27209,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="1740" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1740" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1740">
         <v>2042</v>
       </c>
@@ -27213,7 +27220,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="1741" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1741" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1741">
         <v>2043</v>
       </c>
@@ -27224,7 +27231,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="1742" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1742" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1742">
         <v>2044</v>
       </c>
@@ -27235,7 +27242,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="1743" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1743" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1743">
         <v>2045</v>
       </c>
@@ -27246,7 +27253,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="1744" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1744" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1744">
         <v>2046</v>
       </c>
@@ -27257,7 +27264,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="1745" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1745" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1745">
         <v>2047</v>
       </c>
@@ -27268,7 +27275,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="1746" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1746" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1746">
         <v>2048</v>
       </c>
@@ -27279,7 +27286,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="1747" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1747" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1747">
         <v>2049</v>
       </c>
@@ -27290,7 +27297,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="1748" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1748" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1748">
         <v>2050</v>
       </c>
@@ -27301,7 +27308,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="1749" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1749" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1749">
         <v>2051</v>
       </c>
@@ -27312,7 +27319,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="1750" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1750" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1750">
         <v>2100</v>
       </c>
@@ -27323,7 +27330,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="1751" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1751" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1751">
         <v>2150</v>
       </c>

</xml_diff>